<commit_message>
Se vieron algunas de las modificaiones de la funcion de read_excel
</commit_message>
<xml_diff>
--- a/libs/pruebaProveedores.xlsx
+++ b/libs/pruebaProveedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\python\respaldos\libs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397CFCF9-356A-4729-9261-6FAA4939306C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7BEFEF-FFD3-40F3-8D69-FDE5904C2359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CCFB028-0A87-4D8A-8188-CAE6F5ACF0D3}"/>
   </bookViews>
@@ -403,55 +403,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF849220-1E3D-4B8F-B05D-87E486BC49BD}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>5000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
         <v>20</v>
       </c>
     </row>

</xml_diff>